<commit_message>
sheet "info" was updated
</commit_message>
<xml_diff>
--- a/inst/xlsx/macrounchainedFocusGW-multiple-applications.xlsx
+++ b/inst/xlsx/macrounchainedFocusGW-multiple-applications.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="63">
   <si>
     <t xml:space="preserve">category</t>
   </si>
@@ -83,7 +83,7 @@
     <t xml:space="preserve">text</t>
   </si>
   <si>
-    <t xml:space="preserve">Name of the substance</t>
+    <t xml:space="preserve">Name of the substance. Names don’t need to be unique, but it may be a good idea if they are.</t>
   </si>
   <si>
     <t xml:space="preserve">kfoc</t>
@@ -122,7 +122,7 @@
     <t xml:space="preserve">[°C]</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference temperature at which the DT50 was measured </t>
+    <t xml:space="preserve">Reference temperature at which the half-life was measured </t>
   </si>
   <si>
     <t xml:space="preserve">dt50_pf</t>
@@ -137,19 +137,19 @@
     <t xml:space="preserve">exp_temp_resp</t>
   </si>
   <si>
-    <t xml:space="preserve">exponent of the temperature response and the exponent of the moisture response </t>
+    <t xml:space="preserve">Exponent of the temperature response (effect of temperature on degradation)</t>
   </si>
   <si>
     <t xml:space="preserve">exp_moist_resp</t>
   </si>
   <si>
-    <t xml:space="preserve">Exponent of the temperature response (effect of temperature on degradation)</t>
+    <t xml:space="preserve">Exponent of the moisture response (effect of soil water content on degradation)</t>
   </si>
   <si>
     <t xml:space="preserve">crop_upt_f</t>
   </si>
   <si>
-    <t xml:space="preserve">Exponent of the moisture response (effect of soil water content on degradation)</t>
+    <t xml:space="preserve">Crop uptake factor. Between 0 (no root uptake of the substance) and 1 (passive uptake of the substance with root water uptake)</t>
   </si>
   <si>
     <t xml:space="preserve">diff_coef</t>
@@ -164,25 +164,34 @@
     <t xml:space="preserve">parent_id</t>
   </si>
   <si>
-    <t xml:space="preserve">Only for metabolites. Leave empty for substances that are not the degradation product of another substance. “id” of the parent substance, i.e. the substance that degrades into the metabolite described in this row.</t>
+    <t xml:space="preserve">Only for metabolites. Leave empty for substances that are not the degradation product of another substance. `id` of the parent substance, i.e. the substance that degrades into the metabolite described in this row. For secondary metabolites (and further), the "parent" will also be a metabolite.</t>
   </si>
   <si>
     <t xml:space="preserve">g_per_mol</t>
   </si>
   <si>
-    <t xml:space="preserve">Molar mass [g/mol] of the substance. Only needed when the substance is degrading into a degradation product or is the degradation product of another substance.</t>
+    <t xml:space="preserve">[g/mol]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Molar mass [g/mol] of the substance. Only needed when the substance is degrading into a degradation product or is the degradation product of another substance. Leave empty otherwise.</t>
   </si>
   <si>
     <t xml:space="preserve">g_as_per_ha</t>
   </si>
   <si>
-    <t xml:space="preserve">Application rate (in g substance per hectare) of the substance. Set to 0 g/ha if the substance is a degradation product.</t>
+    <t xml:space="preserve">[g/ha]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application rate (in g substance per hectare) of the substance. Set to 0 g/ha if the substance is a degradation product. In case of several applications per year, give the values separated with a vertical bar (see https://en.wikipedia.org/wiki/Vertical_bar). Do not quote the values. For example, for two applications of 1000g/ha and 90g/ha, respectively, type 1000|900</t>
   </si>
   <si>
     <t xml:space="preserve">app_j_day</t>
   </si>
   <si>
-    <t xml:space="preserve">Application date (in Julian day) of the substance. Use the application date of the applied substance (the parent) if the substance is a degradation product.</t>
+    <t xml:space="preserve">[Julian day]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application date (in Julian day) of the substance. Use the application date of the applied substance (the original parent) if the substance is a degradation product. In case of several applications per year, give the values separated with a vertical bar (see https://en.wikipedia.org/wiki/Vertical_bar). Do not quote the values. For example, for two applications on Julian days 298 and 305, respectively, type 298|305</t>
   </si>
   <si>
     <t xml:space="preserve">transf_f</t>
@@ -288,7 +297,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -305,6 +314,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -314,6 +331,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -389,6 +414,332 @@
 </styleSheet>
 </file>
 
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.1"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="55.05"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10"/>
+    </row>
+    <row r="7" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="69.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="81" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -397,7 +748,7 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -462,13 +813,13 @@
         <v>48</v>
       </c>
       <c r="N1" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="P1" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="P1" s="0" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -476,7 +827,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>172</v>
@@ -509,10 +860,10 @@
         <v>200</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -520,7 +871,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>52</v>
@@ -560,10 +911,10 @@
         <v>0.706666666666667</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>